<commit_message>
can load tests to an excel and use reasoning mistral models
</commit_message>
<xml_diff>
--- a/Adresses_test.xlsx
+++ b/Adresses_test.xlsx
@@ -578,12 +578,12 @@
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>oui</t>
+          <t>non</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -629,12 +629,12 @@
           <t>8 FENCHURCH PLACE</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr">
         <is>
           <t>LEVEL 3</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr">
         <is>
@@ -643,7 +643,7 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>V</t>
         </is>
       </c>
     </row>
@@ -686,7 +686,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>26 PLACE DE LA GARE</t>
+          <t>"26 PLACE DE LA GARE</t>
         </is>
       </c>
       <c r="N4" t="inlineStr"/>
@@ -694,12 +694,12 @@
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>oui</t>
+          <t>oui"</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>F</t>
         </is>
       </c>
     </row>
@@ -810,7 +810,7 @@
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>non</t>
+          <t>oui</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -863,15 +863,15 @@
       </c>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>non</t>
-        </is>
-      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>oui</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>F</t>
         </is>
       </c>
     </row>
@@ -924,20 +924,20 @@
         </is>
       </c>
       <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>CS 70050</t>
+        </is>
+      </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>CS 70050</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
           <t>oui</t>
         </is>
       </c>
+      <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>F</t>
         </is>
       </c>
     </row>
@@ -987,15 +987,15 @@
       </c>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr">
+      <c r="P9" t="inlineStr">
         <is>
           <t>oui</t>
         </is>
       </c>
+      <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>F</t>
         </is>
       </c>
     </row>
@@ -1044,24 +1044,20 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
+          <t>110 ESPLANADE DU GRAL DE GAULLE</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
           <t>TOUR B LA DEFENSE 4</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>TOUR B</t>
-        </is>
-      </c>
       <c r="O10" t="inlineStr">
         <is>
           <t>9EME ETAGE</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>110 ESPLANADE DU GRAL DE GAULLE</t>
-        </is>
-      </c>
+      <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr">
         <is>
           <t>oui</t>
@@ -1069,7 +1065,7 @@
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>V</t>
         </is>
       </c>
     </row>
@@ -1177,15 +1173,15 @@
       </c>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr">
+      <c r="P12" t="inlineStr">
         <is>
           <t>oui</t>
         </is>
       </c>
+      <c r="Q12" t="inlineStr"/>
       <c r="R12" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>F</t>
         </is>
       </c>
     </row>
@@ -1226,24 +1222,25 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>1 RUE JEAN MERMOZ</t>
+          <t>La réponse est :
+1 RUE JEAN MERMOZ</t>
         </is>
       </c>
       <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>ZAE SAINT-GUENAULT</t>
+        </is>
+      </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>ZAE SAINT-GUENAULT</t>
-        </is>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
           <t>oui</t>
         </is>
       </c>
+      <c r="Q13" t="inlineStr"/>
       <c r="R13" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>F</t>
         </is>
       </c>
     </row>
@@ -1297,15 +1294,15 @@
       </c>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>non</t>
-        </is>
-      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>oui</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>F</t>
         </is>
       </c>
     </row>
@@ -1353,15 +1350,15 @@
       </c>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>non</t>
-        </is>
-      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>oui</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr"/>
       <c r="R15" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>F</t>
         </is>
       </c>
     </row>
@@ -1413,15 +1410,15 @@
       </c>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>non</t>
-        </is>
-      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>oui</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>F</t>
         </is>
       </c>
     </row>
@@ -1476,14 +1473,10 @@
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>PCM DEPARTMENT-CFS SETTLEMENTS</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>FOR ATT NICOLA QUADDY</t>
-        </is>
-      </c>
+          <t>60 LONDON WALL</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr">
         <is>
           <t>3RD FLOOR</t>
@@ -1491,7 +1484,7 @@
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>60 LONDON WALL</t>
+          <t>PCM DEPARTMENT-CFS SETTLEMENTS FOR ATT NICOLA QUADDY</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
@@ -1564,12 +1557,12 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>non</t>
+          <t>oui</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>V</t>
         </is>
       </c>
     </row>
@@ -1624,24 +1617,28 @@
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>C/O ING PCM</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr"/>
+          <t>LOCATIECODE AS 04 37</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>POSTBUS 1800</t>
+        </is>
+      </c>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr">
         <is>
-          <t>A LOCATIECODE AS 04 37 POSTBUS 1800</t>
+          <t>C/O ING PCM A</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>non</t>
+          <t>oui</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>F</t>
         </is>
       </c>
     </row>
@@ -1689,15 +1686,15 @@
       </c>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr"/>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>non</t>
-        </is>
-      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>"oui"</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr"/>
       <c r="R20" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>F</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
tried to run a second model after the first one, meh
</commit_message>
<xml_diff>
--- a/Adresses_test.xlsx
+++ b/Adresses_test.xlsx
@@ -578,12 +578,12 @@
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>non</t>
+          <t>oui</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>F</t>
         </is>
       </c>
     </row>
@@ -626,15 +626,15 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>8 FENCHURCH PLACE</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr">
+          <t>Réponse: 8 FENCHURCH PLACE</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
         <is>
           <t>LEVEL 3</t>
         </is>
       </c>
+      <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr">
         <is>
@@ -643,7 +643,7 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>F</t>
         </is>
       </c>
     </row>
@@ -686,7 +686,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>"26 PLACE DE LA GARE</t>
+          <t>26 PLACE DE LA GARE</t>
         </is>
       </c>
       <c r="N4" t="inlineStr"/>
@@ -694,12 +694,12 @@
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>oui"</t>
+          <t>oui</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>V</t>
         </is>
       </c>
     </row>
@@ -863,15 +863,15 @@
       </c>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr">
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr">
         <is>
           <t>oui</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>V</t>
         </is>
       </c>
     </row>
@@ -929,15 +929,15 @@
           <t>CS 70050</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>oui</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>non</t>
+        </is>
+      </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -987,15 +987,15 @@
       </c>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr">
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr">
         <is>
           <t>oui</t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>V</t>
         </is>
       </c>
     </row>
@@ -1060,7 +1060,7 @@
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>oui</t>
+          <t>non</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1173,15 +1173,15 @@
       </c>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr">
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr">
         <is>
           <t>oui</t>
         </is>
       </c>
-      <c r="Q12" t="inlineStr"/>
       <c r="R12" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>V</t>
         </is>
       </c>
     </row>
@@ -1222,25 +1222,24 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>La réponse est :
-1 RUE JEAN MERMOZ</t>
+          <t>1 RUE JEAN MERMOZ</t>
         </is>
       </c>
       <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr">
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr">
         <is>
           <t>ZAE SAINT-GUENAULT</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr">
+      <c r="Q13" t="inlineStr">
         <is>
           <t>oui</t>
         </is>
       </c>
-      <c r="Q13" t="inlineStr"/>
       <c r="R13" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>V</t>
         </is>
       </c>
     </row>
@@ -1294,15 +1293,15 @@
       </c>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr">
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr">
         <is>
           <t>oui</t>
         </is>
       </c>
-      <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>V</t>
         </is>
       </c>
     </row>
@@ -1350,15 +1349,15 @@
       </c>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr">
+      <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr">
         <is>
           <t>oui</t>
         </is>
       </c>
-      <c r="Q15" t="inlineStr"/>
       <c r="R15" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>V</t>
         </is>
       </c>
     </row>
@@ -1410,15 +1409,15 @@
       </c>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr">
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr">
         <is>
           <t>oui</t>
         </is>
       </c>
-      <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>V</t>
         </is>
       </c>
     </row>
@@ -1476,7 +1475,11 @@
           <t>60 LONDON WALL</t>
         </is>
       </c>
-      <c r="N17" t="inlineStr"/>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>PCM DEPARTMENT-CFS SETTLEMENTS</t>
+        </is>
+      </c>
       <c r="O17" t="inlineStr">
         <is>
           <t>3RD FLOOR</t>
@@ -1484,7 +1487,7 @@
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>PCM DEPARTMENT-CFS SETTLEMENTS FOR ATT NICOLA QUADDY</t>
+          <t>FOR ATT NICOLA QUADDY</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
@@ -1550,11 +1553,7 @@
       </c>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr">
-        <is>
-          <t>MME LISA ROBERTSON</t>
-        </is>
-      </c>
+      <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr">
         <is>
           <t>oui</t>
@@ -1562,7 +1561,7 @@
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>F</t>
         </is>
       </c>
     </row>
@@ -1617,28 +1616,24 @@
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>LOCATIECODE AS 04 37</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
           <t>POSTBUS 1800</t>
         </is>
       </c>
+      <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr">
         <is>
-          <t>C/O ING PCM A</t>
+          <t>C/O ING PCM A LOCATIECODE AS 04 37</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>oui</t>
+          <t>non</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>V</t>
         </is>
       </c>
     </row>
@@ -1686,15 +1681,15 @@
       </c>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr">
-        <is>
-          <t>"oui"</t>
-        </is>
-      </c>
-      <c r="Q20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>oui</t>
+        </is>
+      </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>V</t>
         </is>
       </c>
     </row>
@@ -1757,7 +1752,7 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>oui</t>
+          <t>non</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">

</xml_diff>

<commit_message>
no need to close the excel file
</commit_message>
<xml_diff>
--- a/Adresses_test.xlsx
+++ b/Adresses_test.xlsx
@@ -514,10 +514,8 @@
           <t>mention speciale / lieu dit</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Extra_16</t>
-        </is>
+      <c r="Q1" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="R1" s="1" t="n">
         <v>17</v>
@@ -569,21 +567,17 @@
           <t>25 BANK STREET</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr">
         <is>
           <t>CANARY WHARF</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>oui</t>
-        </is>
-      </c>
+      <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>V</t>
         </is>
       </c>
     </row>
@@ -629,21 +623,17 @@
           <t>8 FENCHURCH PLACE</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>LEVEL 3</t>
         </is>
       </c>
+      <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>non</t>
-        </is>
-      </c>
+      <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>F</t>
         </is>
       </c>
     </row>
@@ -692,11 +682,7 @@
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>oui</t>
-        </is>
-      </c>
+      <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr">
         <is>
           <t>V</t>
@@ -752,11 +738,7 @@
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>oui</t>
-        </is>
-      </c>
+      <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr">
         <is>
           <t>V</t>
@@ -808,11 +790,7 @@
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>oui</t>
-        </is>
-      </c>
+      <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr">
         <is>
           <t>V</t>
@@ -864,11 +842,7 @@
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>oui</t>
-        </is>
-      </c>
+      <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr">
         <is>
           <t>V</t>
@@ -930,11 +904,7 @@
           <t>CS 70050</t>
         </is>
       </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>oui</t>
-        </is>
-      </c>
+      <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr">
         <is>
           <t>V</t>
@@ -988,11 +958,7 @@
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>oui</t>
-        </is>
-      </c>
+      <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr">
         <is>
           <t>V</t>
@@ -1044,12 +1010,12 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>92 ESPLANADE DU GRAL DE GAULLE</t>
+          <t>110 ESPLANADE DU GRAL DE GAULLE</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>TOUR B LA DEFENSE 4</t>
+          <t>TOUR</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1057,12 +1023,12 @@
           <t>9EME ETAGE</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>oui</t>
-        </is>
-      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>LA DEFENSE 4 B</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr"/>
       <c r="R10" t="inlineStr">
         <is>
           <t>F</t>
@@ -1116,11 +1082,7 @@
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>oui</t>
-        </is>
-      </c>
+      <c r="Q11" t="inlineStr"/>
       <c r="R11" t="inlineStr">
         <is>
           <t>V</t>
@@ -1174,11 +1136,7 @@
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>oui</t>
-        </is>
-      </c>
+      <c r="Q12" t="inlineStr"/>
       <c r="R12" t="inlineStr">
         <is>
           <t>V</t>
@@ -1232,11 +1190,7 @@
           <t>ZAE SAINT-GUENAULT</t>
         </is>
       </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>oui</t>
-        </is>
-      </c>
+      <c r="Q13" t="inlineStr"/>
       <c r="R13" t="inlineStr">
         <is>
           <t>V</t>
@@ -1294,11 +1248,7 @@
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>oui</t>
-        </is>
-      </c>
+      <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr">
         <is>
           <t>V</t>
@@ -1350,11 +1300,7 @@
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>oui</t>
-        </is>
-      </c>
+      <c r="Q15" t="inlineStr"/>
       <c r="R15" t="inlineStr">
         <is>
           <t>V</t>
@@ -1410,11 +1356,7 @@
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>oui</t>
-        </is>
-      </c>
+      <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr">
         <is>
           <t>V</t>
@@ -1490,14 +1432,10 @@
           <t>FOR ATT NICOLA QUADDY</t>
         </is>
       </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>non</t>
-        </is>
-      </c>
+      <c r="Q17" t="inlineStr"/>
       <c r="R17" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>F</t>
         </is>
       </c>
     </row>
@@ -1553,15 +1491,15 @@
       </c>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>oui</t>
-        </is>
-      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>MME LISA ROBERTSON</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr"/>
       <c r="R18" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>V</t>
         </is>
       </c>
     </row>
@@ -1626,11 +1564,7 @@
           <t>C/O ING PCM A LOCATIECODE AS 04 37</t>
         </is>
       </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>non</t>
-        </is>
-      </c>
+      <c r="Q19" t="inlineStr"/>
       <c r="R19" t="inlineStr">
         <is>
           <t>V</t>
@@ -1682,11 +1616,7 @@
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr"/>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>oui</t>
-        </is>
-      </c>
+      <c r="Q20" t="inlineStr"/>
       <c r="R20" t="inlineStr">
         <is>
           <t>V</t>
@@ -1750,11 +1680,7 @@
           <t>I-20121 MILANO</t>
         </is>
       </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>oui</t>
-        </is>
-      </c>
+      <c r="Q21" t="inlineStr"/>
       <c r="R21" t="inlineStr">
         <is>
           <t>V</t>
@@ -14119,10 +14045,8 @@
       <c r="E221" t="inlineStr"/>
       <c r="F221" t="inlineStr"/>
       <c r="G221" t="inlineStr"/>
-      <c r="H221" t="inlineStr">
-        <is>
-          <t>02390</t>
-        </is>
+      <c r="H221" t="n">
+        <v>2390</v>
       </c>
       <c r="I221" t="inlineStr">
         <is>
@@ -16437,10 +16361,8 @@
           <t>BEVRIJDINGSLAAN 13</t>
         </is>
       </c>
-      <c r="N259" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+      <c r="N259" t="n">
+        <v>15</v>
       </c>
       <c r="O259" t="inlineStr"/>
       <c r="P259" t="inlineStr"/>
@@ -19259,10 +19181,8 @@
           <t>INDUSTRIEWEG 98</t>
         </is>
       </c>
-      <c r="N305" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+      <c r="N305" t="n">
+        <v>100</v>
       </c>
       <c r="O305" t="inlineStr"/>
       <c r="P305" t="inlineStr"/>
@@ -31901,10 +31821,8 @@
       </c>
       <c r="F543" t="inlineStr"/>
       <c r="G543" t="inlineStr"/>
-      <c r="H543" t="inlineStr">
-        <is>
-          <t>06560</t>
-        </is>
+      <c r="H543" t="n">
+        <v>6560</v>
       </c>
       <c r="I543" t="inlineStr">
         <is>
@@ -35787,10 +35705,8 @@
       </c>
       <c r="F625" t="inlineStr"/>
       <c r="G625" t="inlineStr"/>
-      <c r="H625" t="inlineStr">
-        <is>
-          <t>06560</t>
-        </is>
+      <c r="H625" t="n">
+        <v>6560</v>
       </c>
       <c r="I625" t="inlineStr">
         <is>
@@ -43331,10 +43247,8 @@
       <c r="E787" t="inlineStr"/>
       <c r="F787" t="inlineStr"/>
       <c r="G787" t="inlineStr"/>
-      <c r="H787" t="inlineStr">
-        <is>
-          <t>00100</t>
-        </is>
+      <c r="H787" t="n">
+        <v>100</v>
       </c>
       <c r="I787" t="inlineStr">
         <is>
@@ -43379,10 +43293,8 @@
       <c r="E788" t="inlineStr"/>
       <c r="F788" t="inlineStr"/>
       <c r="G788" t="inlineStr"/>
-      <c r="H788" t="inlineStr">
-        <is>
-          <t>02000</t>
-        </is>
+      <c r="H788" t="n">
+        <v>2000</v>
       </c>
       <c r="I788" t="inlineStr">
         <is>
@@ -45659,10 +45571,8 @@
       <c r="E837" t="inlineStr"/>
       <c r="F837" t="inlineStr"/>
       <c r="G837" t="inlineStr"/>
-      <c r="H837" t="inlineStr">
-        <is>
-          <t>09100</t>
-        </is>
+      <c r="H837" t="n">
+        <v>9100</v>
       </c>
       <c r="I837" t="inlineStr">
         <is>
@@ -51817,10 +51727,8 @@
         </is>
       </c>
       <c r="G969" t="inlineStr"/>
-      <c r="H969" t="inlineStr">
-        <is>
-          <t>06510</t>
-        </is>
+      <c r="H969" t="n">
+        <v>6510</v>
       </c>
       <c r="I969" t="inlineStr">
         <is>
@@ -53173,10 +53081,8 @@
       </c>
       <c r="F998" t="inlineStr"/>
       <c r="G998" t="inlineStr"/>
-      <c r="H998" t="inlineStr">
-        <is>
-          <t>06560</t>
-        </is>
+      <c r="H998" t="n">
+        <v>6560</v>
       </c>
       <c r="I998" t="inlineStr">
         <is>
@@ -53741,10 +53647,8 @@
       <c r="E1010" t="inlineStr"/>
       <c r="F1010" t="inlineStr"/>
       <c r="G1010" t="inlineStr"/>
-      <c r="H1010" t="inlineStr">
-        <is>
-          <t>02390</t>
-        </is>
+      <c r="H1010" t="n">
+        <v>2390</v>
       </c>
       <c r="I1010" t="inlineStr">
         <is>
@@ -59289,10 +59193,8 @@
       <c r="E1130" t="inlineStr"/>
       <c r="F1130" t="inlineStr"/>
       <c r="G1130" t="inlineStr"/>
-      <c r="H1130" t="inlineStr">
-        <is>
-          <t>02110</t>
-        </is>
+      <c r="H1130" t="n">
+        <v>2110</v>
       </c>
       <c r="I1130" t="inlineStr">
         <is>
@@ -59341,10 +59243,8 @@
         </is>
       </c>
       <c r="G1131" t="inlineStr"/>
-      <c r="H1131" t="inlineStr">
-        <is>
-          <t>02100</t>
-        </is>
+      <c r="H1131" t="n">
+        <v>2100</v>
       </c>
       <c r="I1131" t="inlineStr">
         <is>
@@ -64869,10 +64769,8 @@
         </is>
       </c>
       <c r="G1246" t="inlineStr"/>
-      <c r="H1246" t="inlineStr">
-        <is>
-          <t>09103</t>
-        </is>
+      <c r="H1246" t="n">
+        <v>9103</v>
       </c>
       <c r="I1246" t="inlineStr">
         <is>

</xml_diff>